<commit_message>
extended moves to all possible (wide, rotations ... )
</commit_message>
<xml_diff>
--- a/test_state.xlsx
+++ b/test_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rotem\PycharmProjects\Roto_DNF_Analyzer\RotoDNF_analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603D1212-3217-4206-BF29-10AE85C90341}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93FB75A-C8DE-4CF7-B7B5-9049FF594260}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{1D16BBEC-8F82-4DE2-BD75-A35ED9AF71E3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="10">
   <si>
     <t>U</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>SOLVED</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -131,13 +140,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>190641</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>125018</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -471,17 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A91CBD5-6D26-42BA-92C3-A7AD9E9E2185}">
-  <dimension ref="A1:BC23"/>
+  <dimension ref="A1:BC25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BB9" sqref="A9:BB9"/>
+      <selection activeCell="A9" sqref="A9:BB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="4" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="53" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="53" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="2.73046875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1486,40 +1493,40 @@
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
       <c r="D7" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
       </c>
       <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1">
         <v>6</v>
       </c>
-      <c r="G7" s="1">
-        <v>7</v>
-      </c>
-      <c r="H7" s="1">
-        <v>8</v>
-      </c>
       <c r="I7" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J7" s="1">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="K7" s="1">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="L7" s="1">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="M7" s="1">
         <v>13</v>
@@ -1531,22 +1538,22 @@
         <v>15</v>
       </c>
       <c r="P7" s="1">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="Q7" s="1">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="R7" s="1">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="S7" s="1">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="T7" s="1">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="U7" s="1">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="V7" s="1">
         <v>22</v>
@@ -1558,49 +1565,49 @@
         <v>24</v>
       </c>
       <c r="Y7" s="1">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="Z7" s="1">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="AA7" s="1">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="AB7" s="1">
+        <v>28</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>29</v>
+      </c>
+      <c r="AD7" s="1">
         <v>30</v>
       </c>
-      <c r="AC7" s="1">
+      <c r="AE7" s="1">
         <v>31</v>
-      </c>
-      <c r="AD7" s="1">
-        <v>28</v>
-      </c>
-      <c r="AE7" s="1">
-        <v>35</v>
       </c>
       <c r="AF7" s="1">
         <v>32</v>
       </c>
       <c r="AG7" s="1">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AH7" s="1">
+        <v>34</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>35</v>
+      </c>
+      <c r="AJ7" s="1">
         <v>36</v>
       </c>
-      <c r="AI7" s="1">
-        <v>33</v>
-      </c>
-      <c r="AJ7" s="1">
-        <v>34</v>
-      </c>
       <c r="AK7" s="1">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="AL7" s="1">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="AM7" s="1">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="AN7" s="1">
         <v>40</v>
@@ -1612,22 +1619,22 @@
         <v>42</v>
       </c>
       <c r="AQ7" s="1">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AR7" s="1">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="AS7" s="1">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="AT7" s="1">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="AU7" s="1">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="AV7" s="1">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AW7" s="1">
         <v>49</v>
@@ -1639,54 +1646,54 @@
         <v>51</v>
       </c>
       <c r="AZ7" s="1">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="BA7" s="1">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="BB7" s="1">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="BC7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
         <v>4</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>8</v>
       </c>
       <c r="E8" s="1">
         <v>5</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1">
         <v>9</v>
       </c>
-      <c r="H8" s="1">
-        <v>6</v>
-      </c>
-      <c r="I8" s="1">
-        <v>3</v>
-      </c>
       <c r="J8" s="1">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="K8" s="1">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="L8" s="1">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="M8" s="1">
         <v>13</v>
@@ -1698,22 +1705,22 @@
         <v>15</v>
       </c>
       <c r="P8" s="1">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="Q8" s="1">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="R8" s="1">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="S8" s="1">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="T8" s="1">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="U8" s="1">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="V8" s="1">
         <v>22</v>
@@ -1725,49 +1732,49 @@
         <v>24</v>
       </c>
       <c r="Y8" s="1">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="Z8" s="1">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="AA8" s="1">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="AB8" s="1">
+        <v>34</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>31</v>
+      </c>
+      <c r="AD8" s="1">
         <v>28</v>
       </c>
-      <c r="AC8" s="1">
-        <v>29</v>
-      </c>
-      <c r="AD8" s="1">
-        <v>30</v>
-      </c>
       <c r="AE8" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AF8" s="1">
         <v>32</v>
       </c>
       <c r="AG8" s="1">
+        <v>29</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>36</v>
+      </c>
+      <c r="AI8" s="1">
         <v>33</v>
       </c>
-      <c r="AH8" s="1">
-        <v>34</v>
-      </c>
-      <c r="AI8" s="1">
-        <v>35</v>
-      </c>
       <c r="AJ8" s="1">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="AK8" s="1">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="AL8" s="1">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="AM8" s="1">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="AN8" s="1">
         <v>40</v>
@@ -1779,22 +1786,22 @@
         <v>42</v>
       </c>
       <c r="AQ8" s="1">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AR8" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="AS8" s="1">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="AT8" s="1">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="AU8" s="1">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="AV8" s="1">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AW8" s="1">
         <v>49</v>
@@ -1806,16 +1813,16 @@
         <v>51</v>
       </c>
       <c r="AZ8" s="1">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="BA8" s="1">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="BB8" s="1">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="BC8" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.45">
@@ -1829,13 +1836,13 @@
         <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E9" s="1">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="F9" s="1">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1">
         <v>7</v>
@@ -1850,7 +1857,7 @@
         <v>10</v>
       </c>
       <c r="K9" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="L9" s="1">
         <v>12</v>
@@ -1859,19 +1866,19 @@
         <v>13</v>
       </c>
       <c r="N9" s="1">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="O9" s="1">
         <v>15</v>
       </c>
       <c r="P9" s="1">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="Q9" s="1">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="R9" s="1">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="S9" s="1">
         <v>19</v>
@@ -1892,46 +1899,46 @@
         <v>24</v>
       </c>
       <c r="Y9" s="1">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="Z9" s="1">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="AA9" s="1">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="AB9" s="1">
+        <v>28</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>29</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>30</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>16</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>14</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>11</v>
+      </c>
+      <c r="AH9" s="1">
         <v>34</v>
       </c>
-      <c r="AC9" s="1">
-        <v>31</v>
-      </c>
-      <c r="AD9" s="1">
-        <v>28</v>
-      </c>
-      <c r="AE9" s="1">
+      <c r="AI9" s="1">
         <v>35</v>
       </c>
-      <c r="AF9" s="1">
-        <v>32</v>
-      </c>
-      <c r="AG9" s="1">
-        <v>29</v>
-      </c>
-      <c r="AH9" s="1">
+      <c r="AJ9" s="1">
         <v>36</v>
-      </c>
-      <c r="AI9" s="1">
-        <v>33</v>
-      </c>
-      <c r="AJ9" s="1">
-        <v>30</v>
       </c>
       <c r="AK9" s="1">
         <v>37</v>
       </c>
       <c r="AL9" s="1">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="AM9" s="1">
         <v>39</v>
@@ -1940,19 +1947,19 @@
         <v>40</v>
       </c>
       <c r="AO9" s="1">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="AP9" s="1">
         <v>42</v>
       </c>
       <c r="AQ9" s="1">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AR9" s="1">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="AS9" s="1">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="AT9" s="1">
         <v>46</v>
@@ -1973,112 +1980,360 @@
         <v>51</v>
       </c>
       <c r="AZ9" s="1">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="BA9" s="1">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="BB9" s="1">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="BC9" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="AJ10" s="3"/>
-      <c r="AK10" s="3"/>
-      <c r="AL10" s="3"/>
-      <c r="AM10" s="3"/>
-      <c r="AN10" s="3"/>
-      <c r="AO10" s="3"/>
-      <c r="AP10" s="3"/>
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1">
+        <v>47</v>
+      </c>
+      <c r="I10" s="1">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1">
+        <v>10</v>
+      </c>
+      <c r="K10" s="1">
+        <v>11</v>
+      </c>
+      <c r="L10" s="1">
+        <v>12</v>
+      </c>
+      <c r="M10" s="1">
+        <v>13</v>
+      </c>
+      <c r="N10" s="1">
+        <v>14</v>
+      </c>
+      <c r="O10" s="1">
+        <v>15</v>
+      </c>
+      <c r="P10" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>17</v>
+      </c>
+      <c r="R10" s="1">
+        <v>18</v>
+      </c>
+      <c r="S10" s="1">
+        <v>19</v>
+      </c>
+      <c r="T10" s="1">
+        <v>2</v>
+      </c>
+      <c r="U10" s="1">
+        <v>21</v>
+      </c>
+      <c r="V10" s="1">
+        <v>22</v>
+      </c>
+      <c r="W10" s="1">
+        <v>5</v>
+      </c>
+      <c r="X10" s="1">
+        <v>24</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>25</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>27</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>28</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>20</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>30</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>31</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>23</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>33</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>34</v>
+      </c>
+      <c r="AI10" s="1">
+        <v>26</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>36</v>
+      </c>
+      <c r="AK10" s="1">
+        <v>37</v>
+      </c>
+      <c r="AL10" s="1">
+        <v>38</v>
+      </c>
+      <c r="AM10" s="1">
+        <v>39</v>
+      </c>
+      <c r="AN10" s="1">
+        <v>40</v>
+      </c>
+      <c r="AO10" s="1">
+        <v>41</v>
+      </c>
+      <c r="AP10" s="1">
+        <v>42</v>
+      </c>
+      <c r="AQ10" s="1">
+        <v>43</v>
+      </c>
+      <c r="AR10" s="1">
+        <v>44</v>
+      </c>
+      <c r="AS10" s="1">
+        <v>45</v>
+      </c>
+      <c r="AT10" s="1">
+        <v>46</v>
+      </c>
+      <c r="AU10" s="1">
+        <v>35</v>
+      </c>
+      <c r="AV10" s="1">
+        <v>48</v>
+      </c>
+      <c r="AW10" s="1">
+        <v>49</v>
+      </c>
+      <c r="AX10" s="1">
+        <v>32</v>
+      </c>
+      <c r="AY10" s="1">
+        <v>51</v>
+      </c>
+      <c r="AZ10" s="1">
+        <v>52</v>
+      </c>
+      <c r="BA10" s="1">
+        <v>29</v>
+      </c>
+      <c r="BB10" s="1">
+        <v>54</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="AJ11" s="4" t="s">
+      <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="AK11" s="4"/>
-      <c r="AL11" s="4"/>
-      <c r="AM11" s="4"/>
-      <c r="AO11" s="4" t="s">
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1">
         <v>5</v>
       </c>
-      <c r="AP11" s="4"/>
-      <c r="AQ11" s="4"/>
-      <c r="AR11" s="4"/>
-      <c r="AT11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU11" s="4"/>
-      <c r="AV11" s="4"/>
-      <c r="AW11" s="4"/>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1">
+        <v>9</v>
+      </c>
+      <c r="J11" s="1">
+        <v>10</v>
+      </c>
+      <c r="K11" s="1">
+        <v>11</v>
+      </c>
+      <c r="L11" s="1">
+        <v>12</v>
+      </c>
+      <c r="M11" s="1">
+        <v>13</v>
+      </c>
+      <c r="N11" s="1">
+        <v>14</v>
+      </c>
+      <c r="O11" s="1">
+        <v>15</v>
+      </c>
+      <c r="P11" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>17</v>
+      </c>
+      <c r="R11" s="1">
+        <v>18</v>
+      </c>
+      <c r="S11" s="1">
+        <v>19</v>
+      </c>
+      <c r="T11" s="1">
+        <v>20</v>
+      </c>
+      <c r="U11" s="1">
+        <v>21</v>
+      </c>
+      <c r="V11" s="1">
+        <v>22</v>
+      </c>
+      <c r="W11" s="1">
+        <v>23</v>
+      </c>
+      <c r="X11" s="1">
+        <v>24</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>25</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>26</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>27</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>28</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>29</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>30</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>31</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>32</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>33</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>34</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>35</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>36</v>
+      </c>
+      <c r="AK11" s="1">
+        <v>37</v>
+      </c>
+      <c r="AL11" s="1">
+        <v>38</v>
+      </c>
+      <c r="AM11" s="1">
+        <v>39</v>
+      </c>
+      <c r="AN11" s="1">
+        <v>40</v>
+      </c>
+      <c r="AO11" s="1">
+        <v>41</v>
+      </c>
+      <c r="AP11" s="1">
+        <v>42</v>
+      </c>
+      <c r="AQ11" s="1">
+        <v>43</v>
+      </c>
+      <c r="AR11" s="1">
+        <v>44</v>
+      </c>
+      <c r="AS11" s="1">
+        <v>45</v>
+      </c>
+      <c r="AT11" s="1">
+        <v>46</v>
+      </c>
+      <c r="AU11" s="1">
+        <v>47</v>
+      </c>
+      <c r="AV11" s="1">
+        <v>48</v>
+      </c>
+      <c r="AW11" s="1">
+        <v>49</v>
+      </c>
+      <c r="AX11" s="1">
+        <v>50</v>
+      </c>
+      <c r="AY11" s="1">
+        <v>51</v>
+      </c>
+      <c r="AZ11" s="1">
+        <v>52</v>
+      </c>
+      <c r="BA11" s="1">
+        <v>53</v>
+      </c>
+      <c r="BB11" s="1">
+        <v>54</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="AJ12">
-        <v>9</v>
-      </c>
-      <c r="AK12">
-        <v>46</v>
-      </c>
-      <c r="AL12">
-        <v>36</v>
-      </c>
-      <c r="AM12">
-        <v>27</v>
-      </c>
-      <c r="AO12">
-        <v>1</v>
-      </c>
-      <c r="AP12">
-        <v>43</v>
-      </c>
-      <c r="AQ12">
-        <v>36</v>
-      </c>
-      <c r="AR12">
-        <v>12</v>
-      </c>
-      <c r="AT12">
-        <v>7</v>
-      </c>
-      <c r="AU12">
-        <v>10</v>
-      </c>
-      <c r="AV12">
-        <v>30</v>
-      </c>
-      <c r="AW12">
-        <v>45</v>
-      </c>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.45">
       <c r="J13" s="2"/>
@@ -2095,42 +2350,24 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-      <c r="AJ13">
-        <v>6</v>
-      </c>
-      <c r="AK13">
-        <v>49</v>
-      </c>
-      <c r="AL13">
-        <v>33</v>
-      </c>
-      <c r="AM13">
-        <v>24</v>
-      </c>
-      <c r="AO13">
+      <c r="AJ13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="4"/>
+      <c r="AM13" s="4"/>
+      <c r="AO13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP13" s="4"/>
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="4"/>
+      <c r="AT13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AP13">
-        <v>40</v>
-      </c>
-      <c r="AQ13">
-        <v>35</v>
-      </c>
-      <c r="AR13">
-        <v>15</v>
-      </c>
-      <c r="AT13">
-        <v>8</v>
-      </c>
-      <c r="AU13">
-        <v>13</v>
-      </c>
-      <c r="AV13">
-        <v>29</v>
-      </c>
-      <c r="AW13">
-        <v>42</v>
-      </c>
+      <c r="AU13" s="4"/>
+      <c r="AV13" s="4"/>
+      <c r="AW13" s="4"/>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.45">
       <c r="J14" s="2"/>
@@ -2148,40 +2385,40 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
       <c r="AJ14">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="AK14">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="AL14">
+        <v>36</v>
+      </c>
+      <c r="AM14">
+        <v>27</v>
+      </c>
+      <c r="AO14">
+        <v>1</v>
+      </c>
+      <c r="AP14">
+        <v>43</v>
+      </c>
+      <c r="AQ14">
+        <v>36</v>
+      </c>
+      <c r="AR14">
+        <v>12</v>
+      </c>
+      <c r="AT14">
+        <v>7</v>
+      </c>
+      <c r="AU14">
+        <v>10</v>
+      </c>
+      <c r="AV14">
         <v>30</v>
       </c>
-      <c r="AM14">
-        <v>21</v>
-      </c>
-      <c r="AO14">
-        <v>3</v>
-      </c>
-      <c r="AP14">
-        <v>37</v>
-      </c>
-      <c r="AQ14">
-        <v>34</v>
-      </c>
-      <c r="AR14">
-        <v>18</v>
-      </c>
-      <c r="AT14">
-        <v>9</v>
-      </c>
-      <c r="AU14">
-        <v>16</v>
-      </c>
-      <c r="AV14">
-        <v>28</v>
-      </c>
       <c r="AW14">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.45">
@@ -2200,40 +2437,40 @@
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
       <c r="AJ15">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AK15">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="AL15">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="AM15">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="AO15">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="AP15">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AQ15">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="AR15">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="AT15">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="AU15">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="AV15">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AW15">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.45">
@@ -2252,40 +2489,40 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="AJ16">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="AK16">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="AL16">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="AM16">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="AO16">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="AP16">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="AQ16">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="AR16">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="AT16">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="AU16">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="AV16">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AW16">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="10:49" x14ac:dyDescent="0.45">
@@ -2303,6 +2540,42 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
+      <c r="AJ17">
+        <v>10</v>
+      </c>
+      <c r="AK17">
+        <v>12</v>
+      </c>
+      <c r="AL17">
+        <v>18</v>
+      </c>
+      <c r="AM17">
+        <v>16</v>
+      </c>
+      <c r="AO17">
+        <v>46</v>
+      </c>
+      <c r="AP17">
+        <v>48</v>
+      </c>
+      <c r="AQ17">
+        <v>54</v>
+      </c>
+      <c r="AR17">
+        <v>52</v>
+      </c>
+      <c r="AT17">
+        <v>19</v>
+      </c>
+      <c r="AU17">
+        <v>21</v>
+      </c>
+      <c r="AV17">
+        <v>27</v>
+      </c>
+      <c r="AW17">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="10:49" x14ac:dyDescent="0.45">
       <c r="J18" s="2"/>
@@ -2319,25 +2592,42 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
-      <c r="AJ18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AK18" s="4"/>
-      <c r="AL18" s="4"/>
-      <c r="AM18" s="4"/>
-      <c r="AN18" s="3"/>
-      <c r="AO18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP18" s="4"/>
-      <c r="AQ18" s="4"/>
-      <c r="AR18" s="4"/>
-      <c r="AT18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU18" s="4"/>
-      <c r="AV18" s="4"/>
-      <c r="AW18" s="4"/>
+      <c r="AJ18">
+        <v>11</v>
+      </c>
+      <c r="AK18">
+        <v>15</v>
+      </c>
+      <c r="AL18">
+        <v>17</v>
+      </c>
+      <c r="AM18">
+        <v>13</v>
+      </c>
+      <c r="AO18">
+        <v>47</v>
+      </c>
+      <c r="AP18">
+        <v>51</v>
+      </c>
+      <c r="AQ18">
+        <v>53</v>
+      </c>
+      <c r="AR18">
+        <v>49</v>
+      </c>
+      <c r="AT18">
+        <v>20</v>
+      </c>
+      <c r="AU18">
+        <v>24</v>
+      </c>
+      <c r="AV18">
+        <v>26</v>
+      </c>
+      <c r="AW18">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" spans="10:49" x14ac:dyDescent="0.45">
       <c r="J19" s="2"/>
@@ -2354,42 +2644,6 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-      <c r="AJ19">
-        <v>1</v>
-      </c>
-      <c r="AK19">
-        <v>19</v>
-      </c>
-      <c r="AL19">
-        <v>28</v>
-      </c>
-      <c r="AM19">
-        <v>54</v>
-      </c>
-      <c r="AO19">
-        <v>25</v>
-      </c>
-      <c r="AP19">
-        <v>16</v>
-      </c>
-      <c r="AQ19">
-        <v>52</v>
-      </c>
-      <c r="AR19">
-        <v>43</v>
-      </c>
-      <c r="AT19">
-        <v>1</v>
-      </c>
-      <c r="AU19">
-        <v>3</v>
-      </c>
-      <c r="AV19">
-        <v>9</v>
-      </c>
-      <c r="AW19">
-        <v>7</v>
-      </c>
     </row>
     <row r="20" spans="10:49" x14ac:dyDescent="0.45">
       <c r="J20" s="2"/>
@@ -2406,42 +2660,25 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
-      <c r="AJ20">
+      <c r="AJ20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AK20">
-        <v>22</v>
-      </c>
-      <c r="AL20">
-        <v>31</v>
-      </c>
-      <c r="AM20">
-        <v>51</v>
-      </c>
-      <c r="AO20">
-        <v>26</v>
-      </c>
-      <c r="AP20">
-        <v>17</v>
-      </c>
-      <c r="AQ20">
-        <v>53</v>
-      </c>
-      <c r="AR20">
-        <v>44</v>
-      </c>
-      <c r="AT20">
-        <v>2</v>
-      </c>
-      <c r="AU20">
-        <v>6</v>
-      </c>
-      <c r="AV20">
-        <v>8</v>
-      </c>
-      <c r="AW20">
-        <v>4</v>
-      </c>
+      <c r="AK20" s="4"/>
+      <c r="AL20" s="4"/>
+      <c r="AM20" s="4"/>
+      <c r="AN20" s="3"/>
+      <c r="AO20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP20" s="4"/>
+      <c r="AQ20" s="4"/>
+      <c r="AR20" s="4"/>
+      <c r="AT20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="4"/>
+      <c r="AV20" s="4"/>
+      <c r="AW20" s="4"/>
     </row>
     <row r="21" spans="10:49" x14ac:dyDescent="0.45">
       <c r="J21" s="2"/>
@@ -2459,126 +2696,230 @@
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
       <c r="AJ21">
+        <v>1</v>
+      </c>
+      <c r="AK21">
+        <v>19</v>
+      </c>
+      <c r="AL21">
+        <v>28</v>
+      </c>
+      <c r="AM21">
+        <v>54</v>
+      </c>
+      <c r="AO21">
+        <v>25</v>
+      </c>
+      <c r="AP21">
+        <v>16</v>
+      </c>
+      <c r="AQ21">
+        <v>52</v>
+      </c>
+      <c r="AR21">
+        <v>43</v>
+      </c>
+      <c r="AT21">
+        <v>1</v>
+      </c>
+      <c r="AU21">
+        <v>3</v>
+      </c>
+      <c r="AV21">
+        <v>9</v>
+      </c>
+      <c r="AW21">
         <v>7</v>
-      </c>
-      <c r="AK21">
-        <v>25</v>
-      </c>
-      <c r="AL21">
-        <v>34</v>
-      </c>
-      <c r="AM21">
-        <v>48</v>
-      </c>
-      <c r="AO21">
-        <v>27</v>
-      </c>
-      <c r="AP21">
-        <v>18</v>
-      </c>
-      <c r="AQ21">
-        <v>54</v>
-      </c>
-      <c r="AR21">
-        <v>45</v>
-      </c>
-      <c r="AT21">
-        <v>46</v>
-      </c>
-      <c r="AU21">
-        <v>10</v>
-      </c>
-      <c r="AV21">
-        <v>19</v>
-      </c>
-      <c r="AW21">
-        <v>37</v>
       </c>
     </row>
     <row r="22" spans="10:49" x14ac:dyDescent="0.45">
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
       <c r="AJ22">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="AK22">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="AL22">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="AM22">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AO22">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AP22">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="AQ22">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="AR22">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="AT22">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="AU22">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="AV22">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="AW22">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="10:49" x14ac:dyDescent="0.45">
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
       <c r="AJ23">
+        <v>7</v>
+      </c>
+      <c r="AK23">
+        <v>25</v>
+      </c>
+      <c r="AL23">
+        <v>34</v>
+      </c>
+      <c r="AM23">
+        <v>48</v>
+      </c>
+      <c r="AO23">
+        <v>27</v>
+      </c>
+      <c r="AP23">
+        <v>18</v>
+      </c>
+      <c r="AQ23">
+        <v>54</v>
+      </c>
+      <c r="AR23">
+        <v>45</v>
+      </c>
+      <c r="AT23">
+        <v>46</v>
+      </c>
+      <c r="AU23">
+        <v>10</v>
+      </c>
+      <c r="AV23">
+        <v>19</v>
+      </c>
+      <c r="AW23">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="10:49" x14ac:dyDescent="0.45">
+      <c r="AJ24">
+        <v>37</v>
+      </c>
+      <c r="AK24">
+        <v>39</v>
+      </c>
+      <c r="AL24">
+        <v>45</v>
+      </c>
+      <c r="AM24">
+        <v>43</v>
+      </c>
+      <c r="AO24">
+        <v>28</v>
+      </c>
+      <c r="AP24">
+        <v>30</v>
+      </c>
+      <c r="AQ24">
+        <v>36</v>
+      </c>
+      <c r="AR24">
+        <v>34</v>
+      </c>
+      <c r="AT24">
+        <v>47</v>
+      </c>
+      <c r="AU24">
+        <v>11</v>
+      </c>
+      <c r="AV24">
+        <v>20</v>
+      </c>
+      <c r="AW24">
         <v>38</v>
       </c>
-      <c r="AK23">
+    </row>
+    <row r="25" spans="10:49" x14ac:dyDescent="0.45">
+      <c r="AJ25">
+        <v>38</v>
+      </c>
+      <c r="AK25">
         <v>42</v>
       </c>
-      <c r="AL23">
+      <c r="AL25">
         <v>44</v>
       </c>
-      <c r="AM23">
+      <c r="AM25">
         <v>40</v>
       </c>
-      <c r="AO23">
+      <c r="AO25">
         <v>29</v>
       </c>
-      <c r="AP23">
+      <c r="AP25">
         <v>33</v>
       </c>
-      <c r="AQ23">
+      <c r="AQ25">
         <v>35</v>
       </c>
-      <c r="AR23">
+      <c r="AR25">
         <v>31</v>
       </c>
-      <c r="AT23">
+      <c r="AT25">
         <v>48</v>
       </c>
-      <c r="AU23">
+      <c r="AU25">
         <v>12</v>
       </c>
-      <c r="AV23">
+      <c r="AV25">
         <v>21</v>
       </c>
-      <c r="AW23">
+      <c r="AW25">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="AT11:AW11"/>
-    <mergeCell ref="AT18:AW18"/>
-    <mergeCell ref="AJ18:AM18"/>
-    <mergeCell ref="AJ11:AM11"/>
-    <mergeCell ref="AO11:AR11"/>
-    <mergeCell ref="AO18:AR18"/>
+    <mergeCell ref="AT13:AW13"/>
+    <mergeCell ref="AT20:AW20"/>
+    <mergeCell ref="AJ20:AM20"/>
+    <mergeCell ref="AJ13:AM13"/>
+    <mergeCell ref="AO13:AR13"/>
+    <mergeCell ref="AO20:AR20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
letter pair in comments work
</commit_message>
<xml_diff>
--- a/test_state.xlsx
+++ b/test_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rotem\PycharmProjects\Roto_DNF_Analyzer\RotoDNF_analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93FB75A-C8DE-4CF7-B7B5-9049FF594260}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506B5017-60B6-43CC-A476-5154B7BE1E93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{1D16BBEC-8F82-4DE2-BD75-A35ED9AF71E3}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:BC25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:BB9"/>
+      <selection activeCell="A9" sqref="A9:BC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1872,10 +1872,10 @@
         <v>15</v>
       </c>
       <c r="P9" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="1">
         <v>6</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>17</v>
       </c>
       <c r="R9" s="1">
         <v>18</v>
@@ -1917,7 +1917,7 @@
         <v>30</v>
       </c>
       <c r="AE9" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AF9" s="1">
         <v>14</v>
@@ -2197,13 +2197,13 @@
         <v>12</v>
       </c>
       <c r="M11" s="1">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="N11" s="1">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="O11" s="1">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P11" s="1">
         <v>16</v>
@@ -2224,13 +2224,13 @@
         <v>21</v>
       </c>
       <c r="V11" s="1">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="W11" s="1">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="X11" s="1">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="Y11" s="1">
         <v>25</v>
@@ -2278,13 +2278,13 @@
         <v>39</v>
       </c>
       <c r="AN11" s="1">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="AO11" s="1">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AP11" s="1">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AQ11" s="1">
         <v>43</v>
@@ -2305,13 +2305,13 @@
         <v>48</v>
       </c>
       <c r="AW11" s="1">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="AX11" s="1">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="AY11" s="1">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="AZ11" s="1">
         <v>52</v>
@@ -2325,15 +2325,6 @@
       <c r="BC11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="AJ12" s="3"/>
-      <c r="AK12" s="3"/>
-      <c r="AL12" s="3"/>
-      <c r="AM12" s="3"/>
-      <c r="AN12" s="3"/>
-      <c r="AO12" s="3"/>
-      <c r="AP12" s="3"/>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.45">
       <c r="J13" s="2"/>

</xml_diff>